<commit_message>
Cleaned up code. Removed DIP getAll fcn as unstable
</commit_message>
<xml_diff>
--- a/Mini Project/C/profiling.xlsx
+++ b/Mini Project/C/profiling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\GitHub\EE580-Assignments\Mini Project\C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ringl\Documents\git\EE580-Assignments\Mini Project\C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4261DB1-2C96-4950-B536-3DE1FB4902B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1069FF-9E61-4B9B-9CDF-E1577CF999F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F88C92FF-84DB-48B4-9434-9AFA54E1C919}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F88C92FF-84DB-48B4-9434-9AFA54E1C919}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,15 +443,15 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F14" activeCellId="1" sqref="D9 F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,7 +470,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -498,7 +498,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -512,7 +512,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -523,7 +523,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -534,7 +534,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -545,7 +545,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1386</v>
       </c>
       <c r="D9">
-        <v>673</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Cleaned up code. Removed DIP getAll fcn as unstable"
This reverts commit 7ac0a68a28ee4868b1c36a8ecc742f41690ab42e.
</commit_message>
<xml_diff>
--- a/Mini Project/C/profiling.xlsx
+++ b/Mini Project/C/profiling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ringl\Documents\git\EE580-Assignments\Mini Project\C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\GitHub\EE580-Assignments\Mini Project\C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1069FF-9E61-4B9B-9CDF-E1577CF999F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4261DB1-2C96-4950-B536-3DE1FB4902B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F88C92FF-84DB-48B4-9434-9AFA54E1C919}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F88C92FF-84DB-48B4-9434-9AFA54E1C919}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,15 +443,15 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" activeCellId="1" sqref="D9 F14"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,7 +470,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -498,7 +498,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -512,7 +512,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -523,7 +523,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -534,7 +534,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -545,7 +545,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1386</v>
       </c>
       <c r="D9">
-        <v>851</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>